<commit_message>
newest edits for document
</commit_message>
<xml_diff>
--- a/results/tmle/SAs/mimic_mortality_nice.xlsx
+++ b/results/tmle/SAs/mimic_mortality_nice.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Tristan/Documents/Projekte/Boston Celi/1 Causal Inference/mit-tmle-cancer/results/tmle/SAs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{174C94DA-D128-174A-A7C1-B639C74F9637}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3252150-1584-454E-B7C3-F36DAD5C12A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="34560" windowHeight="21600"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="mimic_base_mortality_1y" sheetId="1" r:id="rId1"/>
@@ -20,14 +20,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>n</t>
   </si>
   <si>
-    <t>none</t>
-  </si>
-  <si>
     <t>ATE</t>
   </si>
   <si>
@@ -62,12 +59,27 @@
   </si>
   <si>
     <t>Metastasized</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>19,744</t>
+  </si>
+  <si>
+    <t>3,875</t>
+  </si>
+  <si>
+    <t>1,430</t>
+  </si>
+  <si>
+    <t>1,535</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
@@ -401,7 +413,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -531,6 +543,43 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -578,7 +627,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -587,6 +636,15 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="19" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="19" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="44">
     <cellStyle name="20% - Accent1" xfId="21" builtinId="30" customBuiltin="1"/>
@@ -943,11 +1001,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N36"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:N37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCellId="3" sqref="A5:N6 K4:N4 A4:I4 A1:N3"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -970,25 +1028,22 @@
   <sheetData>
     <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4" t="s">
-        <v>2</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="9"/>
+      <c r="D1" s="10"/>
       <c r="F1" s="4"/>
       <c r="G1" s="4"/>
       <c r="H1" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I1" s="4"/>
       <c r="J1" s="4"/>
       <c r="K1" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L1" s="4"/>
       <c r="M1" s="4"/>
@@ -996,232 +1051,219 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A2" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="5" t="s">
+    <row r="2" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="6">
-        <v>0.30399108600000002</v>
-      </c>
-      <c r="F2" s="6">
-        <v>5.8184506184144101E-3</v>
-      </c>
-      <c r="G2" s="6">
-        <v>-1.9868954910937102E-3</v>
-      </c>
-      <c r="H2" s="6">
-        <v>0.29733436499999999</v>
-      </c>
-      <c r="I2" s="6">
-        <v>-1.89103213611786E-3</v>
-      </c>
-      <c r="J2" s="6">
-        <v>-8.5382797279320195E-3</v>
-      </c>
-      <c r="K2" s="6">
-        <v>0.310647807</v>
-      </c>
-      <c r="L2" s="6">
-        <v>1.35279333729467E-2</v>
-      </c>
-      <c r="M2" s="6">
-        <v>4.5644887457446E-3</v>
-      </c>
-      <c r="N2" s="7">
-        <v>19744</v>
-      </c>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
+      <c r="N2" s="4"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="5" t="s">
         <v>8</v>
       </c>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
       <c r="E3" s="6">
-        <v>0.62116128999999998</v>
+        <v>0.30399108600000002</v>
       </c>
       <c r="F3" s="6">
-        <v>-2.2721818760452699E-2</v>
+        <v>5.8184506184144101E-3</v>
       </c>
       <c r="G3" s="6">
-        <v>-9.5124324224995505E-3</v>
+        <v>-1.9868954910937102E-3</v>
       </c>
       <c r="H3" s="6">
-        <v>0.60528570500000001</v>
+        <v>0.29733436499999999</v>
       </c>
       <c r="I3" s="6">
-        <v>-4.1778354105726397E-2</v>
+        <v>-1.89103213611786E-3</v>
       </c>
       <c r="J3" s="6">
-        <v>-2.7232475330681401E-2</v>
+        <v>-8.5382797279320195E-3</v>
       </c>
       <c r="K3" s="6">
-        <v>0.63703687600000003</v>
+        <v>0.310647807</v>
       </c>
       <c r="L3" s="6">
-        <v>-3.6652834151788701E-3</v>
+        <v>1.35279333729467E-2</v>
       </c>
       <c r="M3" s="6">
-        <v>0.01</v>
-      </c>
-      <c r="N3" s="7">
-        <v>3875</v>
+        <v>4.5644887457446E-3</v>
+      </c>
+      <c r="N3" s="7" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>8</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
       <c r="E4" s="6">
-        <v>0.48181818199999998</v>
+        <v>0.62116128999999998</v>
       </c>
       <c r="F4" s="6">
-        <v>-2.7432621088224799E-3</v>
+        <v>-2.2721818760452699E-2</v>
       </c>
       <c r="G4" s="6">
-        <v>1.56225104396345E-2</v>
+        <v>-9.5124324224995505E-3</v>
       </c>
       <c r="H4" s="6">
-        <v>0.45483044099999997</v>
+        <v>0.60528570500000001</v>
       </c>
       <c r="I4" s="6">
-        <v>-3.9717798772305503E-2</v>
+        <v>-4.1778354105726397E-2</v>
       </c>
       <c r="J4" s="6">
-        <v>-1.5875784116234401E-2</v>
+        <v>-2.7232475330681401E-2</v>
       </c>
       <c r="K4" s="6">
-        <v>0.50880592199999997</v>
+        <v>0.63703687600000003</v>
       </c>
       <c r="L4" s="6">
-        <v>3.4231274554660601E-2</v>
+        <v>-3.6652834151788701E-3</v>
       </c>
       <c r="M4" s="6">
-        <v>4.71208049955033E-2</v>
-      </c>
-      <c r="N4" s="7">
-        <v>1430</v>
+        <v>0.01</v>
+      </c>
+      <c r="N4" s="7" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>8</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
       <c r="E5" s="6">
-        <v>0.58241758200000004</v>
+        <v>0.48181818199999998</v>
       </c>
       <c r="F5" s="6">
-        <v>-1.39677122383189E-2</v>
+        <v>-2.7432621088224799E-3</v>
       </c>
       <c r="G5" s="6">
-        <v>-7.2595587195600303E-2</v>
+        <v>1.56225104396345E-2</v>
       </c>
       <c r="H5" s="6">
-        <v>0.54897401899999998</v>
+        <v>0.45483044099999997</v>
       </c>
       <c r="I5" s="6">
-        <v>-5.1089958505831201E-2</v>
+        <v>-3.9717798772305503E-2</v>
       </c>
       <c r="J5" s="6">
-        <v>-0.10652969526355199</v>
+        <v>-1.5875784116234401E-2</v>
       </c>
       <c r="K5" s="6">
-        <v>0.61586114599999997</v>
+        <v>0.50880592199999997</v>
       </c>
       <c r="L5" s="6">
-        <v>2.3154534029193301E-2</v>
+        <v>3.4231274554660601E-2</v>
       </c>
       <c r="M5" s="6">
-        <v>-3.8661479127648599E-2</v>
-      </c>
-      <c r="N5" s="7">
-        <v>910</v>
+        <v>4.71208049955033E-2</v>
+      </c>
+      <c r="N5" s="7" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>8</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
       <c r="E6" s="6">
+        <v>0.58241758200000004</v>
+      </c>
+      <c r="F6" s="6">
+        <v>-1.39677122383189E-2</v>
+      </c>
+      <c r="G6" s="6">
+        <v>-7.2595587195600303E-2</v>
+      </c>
+      <c r="H6" s="6">
+        <v>0.54897401899999998</v>
+      </c>
+      <c r="I6" s="6">
+        <v>-5.1089958505831201E-2</v>
+      </c>
+      <c r="J6" s="6">
+        <v>-0.10652969526355199</v>
+      </c>
+      <c r="K6" s="6">
+        <v>0.61586114599999997</v>
+      </c>
+      <c r="L6" s="6">
+        <v>2.3154534029193301E-2</v>
+      </c>
+      <c r="M6" s="6">
+        <v>-3.8661479127648599E-2</v>
+      </c>
+      <c r="N6" s="7">
+        <v>910</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A7" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="6">
         <v>0.77394136800000002</v>
       </c>
-      <c r="F6" s="6">
+      <c r="F7" s="6">
         <v>-1.7144402355788201E-2</v>
       </c>
-      <c r="G6" s="6">
+      <c r="G7" s="6">
         <v>-9.0455490120829908E-3</v>
       </c>
-      <c r="H6" s="6">
+      <c r="H7" s="6">
         <v>0.75209264300000001</v>
       </c>
-      <c r="I6" s="6">
+      <c r="I7" s="6">
         <v>-4.1524549968492301E-2</v>
       </c>
-      <c r="J6" s="6">
+      <c r="J7" s="6">
         <v>-3.43527873897152E-2</v>
       </c>
-      <c r="K6" s="6">
+      <c r="K7" s="6">
         <v>0.795790094</v>
       </c>
-      <c r="L6" s="6">
+      <c r="L7" s="6">
         <v>7.2357452569159902E-3</v>
       </c>
-      <c r="M6" s="6">
+      <c r="M7" s="6">
         <v>1.6261689365549298E-2</v>
       </c>
-      <c r="N6" s="7">
-        <v>1535</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="L7" s="3"/>
-      <c r="M7" s="3"/>
+      <c r="N7" s="7" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="F8" s="3"/>
@@ -1231,54 +1273,51 @@
       <c r="M8" s="3"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="E9" s="3"/>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
       <c r="I9" s="3"/>
-      <c r="K9" s="3"/>
       <c r="L9" s="3"/>
       <c r="M9" s="3"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
-      <c r="K14" s="3"/>
-      <c r="L14" s="3"/>
-      <c r="M14" s="3"/>
-    </row>
-    <row r="17" spans="5:13" x14ac:dyDescent="0.2">
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
-      <c r="K17" s="3"/>
-      <c r="L17" s="3"/>
-      <c r="M17" s="3"/>
-    </row>
-    <row r="20" spans="5:13" x14ac:dyDescent="0.2">
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
-      <c r="I20" s="3"/>
-      <c r="K20" s="3"/>
-      <c r="L20" s="3"/>
-      <c r="M20" s="3"/>
-    </row>
-    <row r="22" spans="5:13" x14ac:dyDescent="0.2">
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
-      <c r="H22" s="3"/>
-      <c r="I22" s="3"/>
-      <c r="K22" s="3"/>
-      <c r="L22" s="3"/>
-      <c r="M22" s="3"/>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="3"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="K15" s="3"/>
+      <c r="L15" s="3"/>
+      <c r="M15" s="3"/>
+    </row>
+    <row r="18" spans="5:13" x14ac:dyDescent="0.2">
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+      <c r="K18" s="3"/>
+      <c r="L18" s="3"/>
+      <c r="M18" s="3"/>
+    </row>
+    <row r="21" spans="5:13" x14ac:dyDescent="0.2">
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3"/>
+      <c r="K21" s="3"/>
+      <c r="L21" s="3"/>
+      <c r="M21" s="3"/>
     </row>
     <row r="23" spans="5:13" x14ac:dyDescent="0.2">
       <c r="E23" s="3"/>
@@ -1420,7 +1459,20 @@
       <c r="L36" s="3"/>
       <c r="M36" s="3"/>
     </row>
+    <row r="37" spans="5:13" x14ac:dyDescent="0.2">
+      <c r="E37" s="3"/>
+      <c r="F37" s="3"/>
+      <c r="G37" s="3"/>
+      <c r="H37" s="3"/>
+      <c r="I37" s="3"/>
+      <c r="K37" s="3"/>
+      <c r="L37" s="3"/>
+      <c r="M37" s="3"/>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:D1"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>